<commit_message>
Some variants for analysis
</commit_message>
<xml_diff>
--- a/hw2/results.xlsx
+++ b/hw2/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="974" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -199,7 +199,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
Added results in results.xlsx
</commit_message>
<xml_diff>
--- a/hw2/results.xlsx
+++ b/hw2/results.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>Graph</t>
   </si>
@@ -29,6 +29,9 @@
     <t>Metis</t>
   </si>
   <si>
+    <t>Metis with no ncuts restriction</t>
+  </si>
+  <si>
     <t>CNM</t>
   </si>
   <si>
@@ -41,7 +44,7 @@
     <t>R=3</t>
   </si>
   <si>
-    <t>ncut=</t>
+    <t>Part=100</t>
   </si>
   <si>
     <t>GrQc</t>
@@ -59,28 +62,115 @@
     <t>Time Taken</t>
   </si>
   <si>
+    <t>15.184s</t>
+  </si>
+  <si>
+    <t>12.729s</t>
+  </si>
+  <si>
+    <t>13.769s</t>
+  </si>
+  <si>
+    <t>0.188s</t>
+  </si>
+  <si>
     <t>0.35s</t>
   </si>
   <si>
     <t>Facebook</t>
   </si>
   <si>
+    <t>0.758s</t>
+  </si>
+  <si>
+    <t>22.563s</t>
+  </si>
+  <si>
+    <t>20.189s</t>
+  </si>
+  <si>
+    <t>0.159s</t>
+  </si>
+  <si>
     <t>0.94s</t>
   </si>
   <si>
     <t>Wiki</t>
   </si>
   <si>
+    <t>22.53s</t>
+  </si>
+  <si>
+    <t>132.213s</t>
+  </si>
+  <si>
+    <t>205.976s</t>
+  </si>
+  <si>
+    <t>0.579s</t>
+  </si>
+  <si>
     <t>4.3s</t>
   </si>
   <si>
     <t>Gnutella</t>
   </si>
   <si>
+    <t>13.852s</t>
+  </si>
+  <si>
+    <t>88.496s</t>
+  </si>
+  <si>
+    <t>110.498s</t>
+  </si>
+  <si>
+    <t>0.148s</t>
+  </si>
+  <si>
     <t>0.96s</t>
   </si>
   <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>2476.892s</t>
+  </si>
+  <si>
+    <t>12.379s</t>
+  </si>
+  <si>
     <t>Entropy</t>
+  </si>
+  <si>
+    <t>For same size of ncuts but varying partition size only for youtube</t>
+  </si>
+  <si>
+    <t>Part=50</t>
+  </si>
+  <si>
+    <t>Part = 75</t>
+  </si>
+  <si>
+    <t>Part= 2</t>
+  </si>
+  <si>
+    <t>Part = 1000</t>
+  </si>
+  <si>
+    <t>11.194s</t>
+  </si>
+  <si>
+    <t>9.125s</t>
+  </si>
+  <si>
+    <t>9.911s</t>
+  </si>
+  <si>
+    <t>3.383s</t>
+  </si>
+  <si>
+    <t>20.417s</t>
   </si>
 </sst>
 </file>
@@ -162,7 +252,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -176,7 +266,23 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -196,10 +302,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -221,188 +327,439 @@
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="1" t="s">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
+      <c r="A3" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>89</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>130</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>146</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="0" t="s">
         <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>85</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>97</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>26</v>
+      </c>
+      <c r="G12" s="5" t="n">
+        <v>315</v>
+      </c>
+      <c r="H12" s="5" t="n">
+        <v>548</v>
+      </c>
+      <c r="I12" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="G16" s="5" t="n">
+        <v>443</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>528</v>
+      </c>
+      <c r="I16" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I18" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F20" s="5" t="n">
+        <v>263</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7"/>
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7"/>
+      <c r="B30" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7"/>
+      <c r="B31" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="A3:A6"/>
@@ -410,6 +767,8 @@
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A23"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A28:A31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>